<commit_message>
Übergeordnetes Ziel in DA-Idee
</commit_message>
<xml_diff>
--- a/Projectmanagement/HTLLEDiplomarbeitsidee_Gekle_Kampl_Schrempf.xlsx
+++ b/Projectmanagement/HTLLEDiplomarbeitsidee_Gekle_Kampl_Schrempf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leobenhtl-my.sharepoint.com/personal/201wita20_o365_htl-leoben_at/Documents/Contrude/Projektmanagement/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\Contrude\Projectmanagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{C0566BD4-94F8-4D5B-A10E-775093E35D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08D665B5-D00C-4D52-A585-29EF2C4AD0C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BA6F1D-CCE3-47F4-9C59-FC1206A5DAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,11 +102,6 @@
     <t>Ziele</t>
   </si>
   <si>
-    <t>1) Verminderung der Falschplatzierung von Containern wegen Kranverschiebung
-2) Ermöglichung der Verfolgung von Container während des Überseetransports
-3) Lesen der Umweltdaten vor und während des Transportprozesses rund um den Container</t>
-  </si>
-  <si>
     <t>Mögliche Ergebnisse</t>
   </si>
   <si>
@@ -153,6 +148,12 @@
   </si>
   <si>
     <t>Contrude (Tracking &amp; Umweltdatenauslesung von Containern)</t>
+  </si>
+  <si>
+    <t>Bau eines Prototypens und Bereitstellung der Software. Die folgenden Funktionen sollen erfüllt werden:
+1.	Verminderung der Falschplatzierung von Containern wegen Kranverschiebung
+2.	Ermöglichung der Verfolgung von Container während des Überseetransports
+3.	Lesen der Umweltdaten vor und während des Transportprozesses rund um den Container</t>
   </si>
 </sst>
 </file>
@@ -423,7 +424,33 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -432,7 +459,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -449,71 +476,18 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -539,6 +513,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -931,7 +932,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -959,24 +960,24 @@
       <c r="H5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="43">
+      <c r="I5" s="24">
         <f ca="1">TODAY()</f>
-        <v>45345</v>
-      </c>
-      <c r="J5" s="43"/>
+        <v>45348</v>
+      </c>
+      <c r="J5" s="24"/>
     </row>
     <row r="6" spans="1:10" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="45" t="s">
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="46"/>
+      <c r="G6" s="35"/>
       <c r="H6" s="7"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -994,44 +995,44 @@
       <c r="J7" s="10"/>
     </row>
     <row r="8" spans="1:10" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="17"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="27"/>
     </row>
     <row r="9" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="26"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
@@ -1046,44 +1047,44 @@
       <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="20"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="30"/>
     </row>
     <row r="14" spans="1:10" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="23"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="33"/>
     </row>
     <row r="15" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
@@ -1098,44 +1099,44 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="20"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="30"/>
     </row>
     <row r="18" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="21"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="23"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="33"/>
     </row>
     <row r="19" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11"/>
@@ -1150,56 +1151,56 @@
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="19"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="19"/>
-      <c r="J21" s="20"/>
+      <c r="A21" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="30"/>
     </row>
     <row r="22" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="36"/>
+      <c r="A22" s="53"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
     </row>
     <row r="23" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="23"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
     </row>
     <row r="24" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
@@ -1214,492 +1215,503 @@
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="17"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
     </row>
     <row r="26" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A26" s="33" t="s">
+      <c r="A26" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="26"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="16"/>
     </row>
     <row r="27" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="29"/>
+      <c r="A27" s="50"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="52"/>
     </row>
     <row r="28" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
-      <c r="J28" s="29"/>
+      <c r="A28" s="50"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="51"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="51"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="51"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="52"/>
     </row>
     <row r="29" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
-      <c r="B29" s="28"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="29"/>
+      <c r="A29" s="50"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="52"/>
     </row>
     <row r="30" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="27"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
-      <c r="J30" s="29"/>
+      <c r="A30" s="50"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="27"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="29"/>
+      <c r="A31" s="50"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
-      <c r="J32" s="29"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="51"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="52"/>
     </row>
     <row r="33" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="51"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="52"/>
     </row>
     <row r="34" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="32"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="19"/>
     </row>
     <row r="35" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="36" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
-      <c r="J36" s="41"/>
+      <c r="B36" s="36"/>
+      <c r="C36" s="36"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="37"/>
     </row>
     <row r="37" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="26"/>
+      <c r="A37" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="16"/>
     </row>
     <row r="38" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="28"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="29"/>
+      <c r="A38" s="50"/>
+      <c r="B38" s="51"/>
+      <c r="C38" s="51"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
+      <c r="I38" s="51"/>
+      <c r="J38" s="52"/>
     </row>
     <row r="39" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="28"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="28"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="29"/>
+      <c r="A39" s="50"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="52"/>
     </row>
     <row r="40" spans="1:10" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="30"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="32"/>
+      <c r="A40" s="17"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="19"/>
     </row>
     <row r="41" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="B42" s="40"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="41"/>
+      <c r="A42" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="36"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="37"/>
     </row>
     <row r="43" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="26"/>
+      <c r="A43" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B43" s="15"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="16"/>
     </row>
     <row r="44" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
-      <c r="B44" s="28"/>
-      <c r="C44" s="28"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="29"/>
+      <c r="A44" s="50"/>
+      <c r="B44" s="51"/>
+      <c r="C44" s="51"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A45" s="27"/>
-      <c r="B45" s="28"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="29"/>
+      <c r="A45" s="50"/>
+      <c r="B45" s="51"/>
+      <c r="C45" s="51"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="51"/>
+      <c r="H45" s="51"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="31"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="32"/>
+      <c r="A46" s="17"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="19"/>
     </row>
     <row r="47" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="41"/>
+      <c r="A48" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="37"/>
     </row>
     <row r="49" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="B49" s="47"/>
-      <c r="C49" s="47"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="47"/>
-      <c r="I49" s="47"/>
-      <c r="J49" s="48"/>
+      <c r="A49" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="38"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="38"/>
+      <c r="F49" s="38"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="38"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="39"/>
       <c r="K49" s="13"/>
     </row>
     <row r="50" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="51"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="41"/>
+      <c r="H50" s="41"/>
+      <c r="I50" s="41"/>
+      <c r="J50" s="42"/>
     </row>
     <row r="51" spans="1:11" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="52"/>
-      <c r="B51" s="53"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="54"/>
+      <c r="A51" s="43"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="44"/>
+      <c r="E51" s="44"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="44"/>
+      <c r="H51" s="44"/>
+      <c r="I51" s="44"/>
+      <c r="J51" s="45"/>
     </row>
     <row r="52" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B53" s="21"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
+      <c r="E53" s="21"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
+      <c r="J53" s="22"/>
+    </row>
+    <row r="54" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A54" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="38"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="38"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
-      <c r="H53" s="38"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="39"/>
-    </row>
-    <row r="54" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="26"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="15"/>
+      <c r="D54" s="15"/>
+      <c r="E54" s="15"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="15"/>
+      <c r="H54" s="15"/>
+      <c r="I54" s="15"/>
+      <c r="J54" s="16"/>
     </row>
     <row r="55" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
-      <c r="H55" s="28"/>
-      <c r="I55" s="28"/>
-      <c r="J55" s="29"/>
+      <c r="A55" s="50"/>
+      <c r="B55" s="51"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
+      <c r="E55" s="51"/>
+      <c r="F55" s="51"/>
+      <c r="G55" s="51"/>
+      <c r="H55" s="51"/>
+      <c r="I55" s="51"/>
+      <c r="J55" s="52"/>
     </row>
     <row r="56" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A56" s="27"/>
-      <c r="B56" s="28"/>
-      <c r="C56" s="28"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="28"/>
-      <c r="F56" s="28"/>
-      <c r="G56" s="28"/>
-      <c r="H56" s="28"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="29"/>
+      <c r="A56" s="50"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
+      <c r="E56" s="51"/>
+      <c r="F56" s="51"/>
+      <c r="G56" s="51"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="52"/>
     </row>
     <row r="57" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="31"/>
-      <c r="G57" s="31"/>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-      <c r="J57" s="32"/>
+      <c r="A57" s="17"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="19"/>
     </row>
     <row r="58" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="22"/>
+    </row>
+    <row r="60" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="B59" s="38"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="38"/>
-      <c r="E59" s="38"/>
-      <c r="F59" s="38"/>
-      <c r="G59" s="38"/>
-      <c r="H59" s="38"/>
-      <c r="I59" s="38"/>
-      <c r="J59" s="39"/>
-    </row>
-    <row r="60" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="31"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="31"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="32"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="19"/>
     </row>
     <row r="61" spans="1:11" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62" s="38"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="38"/>
-      <c r="E62" s="38"/>
-      <c r="F62" s="38"/>
-      <c r="G62" s="38"/>
-      <c r="H62" s="38"/>
-      <c r="I62" s="38"/>
-      <c r="J62" s="39"/>
+      <c r="A62" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="21"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
+      <c r="J62" s="22"/>
     </row>
     <row r="63" spans="1:11" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A63" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="25"/>
-      <c r="D63" s="25"/>
-      <c r="E63" s="25"/>
-      <c r="F63" s="25"/>
-      <c r="G63" s="25"/>
-      <c r="H63" s="25"/>
-      <c r="I63" s="25"/>
-      <c r="J63" s="26"/>
+      <c r="A63" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15"/>
+      <c r="D63" s="15"/>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="15"/>
+      <c r="H63" s="15"/>
+      <c r="I63" s="15"/>
+      <c r="J63" s="16"/>
       <c r="K63" s="13"/>
     </row>
     <row r="64" spans="1:11" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="30"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="31"/>
-      <c r="F64" s="31"/>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-      <c r="J64" s="32"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="19"/>
     </row>
     <row r="65" spans="1:10" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+      <c r="F66" s="21"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
+      <c r="J66" s="22"/>
+    </row>
+    <row r="67" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A67" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B66" s="38"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="38"/>
-      <c r="E66" s="38"/>
-      <c r="F66" s="38"/>
-      <c r="G66" s="38"/>
-      <c r="H66" s="38"/>
-      <c r="I66" s="38"/>
-      <c r="J66" s="39"/>
-    </row>
-    <row r="67" spans="1:10" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A67" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" s="25"/>
-      <c r="C67" s="25"/>
-      <c r="D67" s="25"/>
-      <c r="E67" s="25"/>
-      <c r="F67" s="25"/>
-      <c r="G67" s="25"/>
-      <c r="H67" s="25"/>
-      <c r="I67" s="25"/>
-      <c r="J67" s="26"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15"/>
+      <c r="D67" s="15"/>
+      <c r="E67" s="15"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="15"/>
+      <c r="H67" s="15"/>
+      <c r="I67" s="15"/>
+      <c r="J67" s="16"/>
     </row>
     <row r="68" spans="1:10" ht="55.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="30"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="31"/>
-      <c r="E68" s="31"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="31"/>
-      <c r="H68" s="31"/>
-      <c r="I68" s="31"/>
-      <c r="J68" s="32"/>
+      <c r="A68" s="17"/>
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="18"/>
+      <c r="F68" s="18"/>
+      <c r="G68" s="18"/>
+      <c r="H68" s="18"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A17:J18"/>
+    <mergeCell ref="A54:J57"/>
+    <mergeCell ref="A26:J34"/>
+    <mergeCell ref="A21:J23"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A53:J53"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A43:J46"/>
+    <mergeCell ref="A37:J40"/>
     <mergeCell ref="A63:J64"/>
     <mergeCell ref="A66:J66"/>
     <mergeCell ref="A67:J68"/>
@@ -1716,17 +1728,6 @@
     <mergeCell ref="A59:J59"/>
     <mergeCell ref="A60:J60"/>
     <mergeCell ref="A62:J62"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A17:J18"/>
-    <mergeCell ref="A54:J57"/>
-    <mergeCell ref="A26:J34"/>
-    <mergeCell ref="A21:J23"/>
-    <mergeCell ref="A25:J25"/>
-    <mergeCell ref="A53:J53"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A43:J46"/>
-    <mergeCell ref="A37:J40"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.78740157480314965" right="0.19685039370078741" top="0" bottom="0.47244094488188981" header="0.51181102362204722" footer="0.35433070866141736"/>
@@ -1739,23 +1740,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1a2ca174-3ffa-4801-8f05-6cc015117562" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005F460AD6521AC94094D79EF685B712E2" ma:contentTypeVersion="15" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ab67fb0d09ec06ffd645cd3a89c74be5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="8c5829c6-aac1-4f1e-b1e2-fbed17fe0519" xmlns:ns4="1a2ca174-3ffa-4801-8f05-6cc015117562" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efeca6be1e9c5ab1d8f8aca2782dd786" ns3:_="" ns4:_="">
     <xsd:import namespace="8c5829c6-aac1-4f1e-b1e2-fbed17fe0519"/>
@@ -1990,32 +1974,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19370120-31E3-4051-AC52-429A5DD579EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1a2ca174-3ffa-4801-8f05-6cc015117562"/>
-    <ds:schemaRef ds:uri="8c5829c6-aac1-4f1e-b1e2-fbed17fe0519"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E20F5023-DB2D-487E-9F38-B71FDF09F2F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1a2ca174-3ffa-4801-8f05-6cc015117562" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFA16C54-A834-4DE9-849F-2CD366592C77}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2032,4 +2008,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E20F5023-DB2D-487E-9F38-B71FDF09F2F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19370120-31E3-4051-AC52-429A5DD579EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1a2ca174-3ffa-4801-8f05-6cc015117562"/>
+    <ds:schemaRef ds:uri="8c5829c6-aac1-4f1e-b1e2-fbed17fe0519"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>